<commit_message>
Added input identifier verification test; updated the data sheet; added allure report
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DESKTOP_WEB/Connect/SegmentsTestData.xlsx
+++ b/src/test/resources/data/DESKTOP_WEB/Connect/SegmentsTestData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>CreateNewSegment</t>
   </si>
@@ -22,25 +22,95 @@
     <t>Password</t>
   </si>
   <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>DataCollections</t>
+  </si>
+  <si>
+    <t>OptionsOfInputIdentifiers</t>
+  </si>
+  <si>
+    <t>InputIdentifiers</t>
+  </si>
+  <si>
+    <t>OptionsOfOutputIdentifiers</t>
+  </si>
+  <si>
+    <t>OutputIdentifiers</t>
+  </si>
+  <si>
+    <t>ExtendFirstPartyAudience</t>
+  </si>
+  <si>
+    <t>Destinations</t>
+  </si>
+  <si>
     <t>vignesh.paramasivam@zeotap.com</t>
   </si>
   <si>
     <t>Zeotap@123</t>
+  </si>
+  <si>
+    <t>ZEOTAP</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>test-ms-01;e2e-QA-Test-01</t>
+  </si>
+  <si>
+    <t>Email;Mobile</t>
+  </si>
+  <si>
+    <t>Google Cookie;MAID;mPlatform</t>
+  </si>
+  <si>
+    <t>Google Cookie;MAID</t>
+  </si>
+  <si>
+    <t>Activate Zeotap Graph</t>
+  </si>
+  <si>
+    <t>Test_Liveramp;testdest</t>
+  </si>
+  <si>
+    <t>ValidateInputIdentifier</t>
+  </si>
+  <si>
+    <t>Email;Mobile;Invalid-Identifier-Here</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -57,15 +127,30 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -283,9 +368,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.43"/>
-    <col customWidth="1" min="2" max="2" width="35.14"/>
-    <col customWidth="1" min="3" max="3" width="24.43"/>
+    <col customWidth="1" min="1" max="1" width="19.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -298,16 +381,169 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
+      <c r="A2" s="4"/>
       <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E5" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="F5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="4"/>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+  </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified test data; Added hack to load page in navigate method
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DESKTOP_WEB/Connect/SegmentsTestData.xlsx
+++ b/src/test/resources/data/DESKTOP_WEB/Connect/SegmentsTestData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>CreateNewSegment</t>
   </si>
@@ -55,31 +55,34 @@
     <t>Zeotap@123</t>
   </si>
   <si>
+    <t>MT AUTOMATION</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>mt_dc_esp</t>
+  </si>
+  <si>
+    <t>Email;Mobile</t>
+  </si>
+  <si>
+    <t>Google Cookie;MAID</t>
+  </si>
+  <si>
+    <t>Activate Zeotap Graph</t>
+  </si>
+  <si>
+    <t>Test Destination</t>
+  </si>
+  <si>
+    <t>ValidateInputIdentifier</t>
+  </si>
+  <si>
     <t>ZEOTAP</t>
   </si>
   <si>
-    <t>Spain</t>
-  </si>
-  <si>
     <t>test-ms-01;e2e-QA-Test-01</t>
-  </si>
-  <si>
-    <t>Email;Mobile</t>
-  </si>
-  <si>
-    <t>Google Cookie;MAID;mPlatform</t>
-  </si>
-  <si>
-    <t>Google Cookie;MAID</t>
-  </si>
-  <si>
-    <t>Activate Zeotap Graph</t>
-  </si>
-  <si>
-    <t>Test_Liveramp;testdest</t>
-  </si>
-  <si>
-    <t>ValidateInputIdentifier</t>
   </si>
   <si>
     <t>Email;Mobile;Invalid-Identifier-Here</t>
@@ -436,13 +439,13 @@
         <v>18</v>
       </c>
       <c r="J2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3">
@@ -475,7 +478,7 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>1</v>
@@ -509,16 +512,16 @@
         <v>13</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>

</xml_diff>